<commit_message>
planning update et changements
Les changements sont fait en suivant les conseils de la prof
</commit_message>
<xml_diff>
--- a/Docs/Planning projet TUT.xlsx
+++ b/Docs/Planning projet TUT.xlsx
@@ -58,31 +58,31 @@
     <t>Tâches</t>
   </si>
   <si>
-    <t>Définition des prérequis pour la marche et l'équilibre du robot</t>
-  </si>
-  <si>
-    <t>Coordination des étapes du déplacement et des membres du robot</t>
-  </si>
-  <si>
-    <t>Début du test de code pour l'équilibre</t>
-  </si>
-  <si>
-    <t>Développement du code pour le déplacement du robot sur un terrain variable</t>
-  </si>
-  <si>
-    <t>Développement de code d'autres comportement sur le robot</t>
-  </si>
-  <si>
     <t>Implementation d'un code pour relever le robot lorsqu'il tombe</t>
   </si>
   <si>
-    <t>Correction des bugs et optimisation du code + Bilan sur la marche du robot</t>
-  </si>
-  <si>
     <t>Maîtrise de l'équilibre statique du robot et des logiciels</t>
   </si>
   <si>
-    <t>Prise en charge d'un poids plat sur le robot sur terrain plat</t>
+    <t>Plannification de scénario pour tester le robot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementation du code pour la marche du robot </t>
+  </si>
+  <si>
+    <t>Scénario sur le déplacement en terrain plat du robot</t>
+  </si>
+  <si>
+    <t>implementation du code pour la marche du robot en terrain accidenté ou pentu.</t>
+  </si>
+  <si>
+    <t>implementation du code pour validé les scénario plus complexes sur le robot (éviter obstacle et / ou galoper)</t>
+  </si>
+  <si>
+    <t>Prise en charge d'un poid sur le robot sur terrain plat et pentu</t>
+  </si>
+  <si>
+    <t>Implementation du code et assemblement du code pour répondre aux attentes de tous les scénarios en même temps</t>
   </si>
 </sst>
 </file>
@@ -601,28 +601,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
@@ -631,125 +628,137 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1058,7 +1067,7 @@
   <dimension ref="B1:Q20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17:G18"/>
+      <selection activeCell="C19" sqref="C19:G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1068,202 +1077,195 @@
   <sheetData>
     <row r="1" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="47"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="21"/>
     </row>
     <row r="3" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="39" t="s">
+      <c r="C4" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="41"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="32"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="35"/>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B6" s="26"/>
+      <c r="C6" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="24"/>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B7" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="38"/>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B8" s="9"/>
+      <c r="C8" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="29"/>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="12"/>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="13"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="15"/>
+    </row>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="38"/>
+    </row>
+    <row r="12" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="18"/>
-    </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B6" s="19"/>
-      <c r="C6" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="22"/>
-    </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B7" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B8" s="10"/>
-      <c r="C8" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="7"/>
-    </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B9" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="26"/>
-    </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B10" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="27"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="29"/>
-    </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B11" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="33"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="41"/>
     </row>
     <row r="13" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="42" t="s">
+      <c r="B14" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="43"/>
-      <c r="D14" s="43"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="44"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="18"/>
     </row>
     <row r="15" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="38" t="s">
+      <c r="B16" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="39" t="s">
+      <c r="C16" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="40"/>
-      <c r="E16" s="40"/>
-      <c r="F16" s="40"/>
-      <c r="G16" s="41"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="32"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="34" t="s">
+      <c r="B17" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17" s="36"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="37"/>
+      <c r="C17" s="42" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="43"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="44"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="23" t="s">
+      <c r="B18" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="27"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="29"/>
+      <c r="C18" s="45"/>
+      <c r="D18" s="46"/>
+      <c r="E18" s="46"/>
+      <c r="F18" s="46"/>
+      <c r="G18" s="47"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="14"/>
+      <c r="C19" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="49"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="49"/>
+      <c r="G19" s="50"/>
     </row>
     <row r="20" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="48"/>
-      <c r="D20" s="49"/>
-      <c r="E20" s="49"/>
-      <c r="F20" s="49"/>
-      <c r="G20" s="50"/>
+      <c r="C20" s="51"/>
+      <c r="D20" s="52"/>
+      <c r="E20" s="52"/>
+      <c r="F20" s="52"/>
+      <c r="G20" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C9:G10"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C8:G8"/>
     <mergeCell ref="C17:G18"/>
     <mergeCell ref="C19:G20"/>
     <mergeCell ref="C4:G4"/>
@@ -1272,6 +1274,13 @@
     <mergeCell ref="C7:G7"/>
     <mergeCell ref="C11:G11"/>
     <mergeCell ref="C12:G12"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C9:G10"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C8:G8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>